<commit_message>
[Doc] Add port C
</commit_message>
<xml_diff>
--- a/MemMap.xlsx
+++ b/MemMap.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6d428188c4adbc4b/Bureau/Hearc/Di Applied/NanoProc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6d428188c4adbc4b/Bureau/Project/NanoProcessor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="61" documentId="11_AD4DB114E441178AC67DF437FE92CEEE683EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A15A0FFD-3F96-47B1-ADB9-317A8D16DEFC}"/>
+  <xr:revisionPtr revIDLastSave="67" documentId="11_AD4DB114E441178AC67DF437FE92CEEE683EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6D07B3D1-2F6F-4A75-810E-47743949BB4D}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>0x00</t>
   </si>
@@ -70,6 +70,12 @@
   </si>
   <si>
     <t>Plan mémoire</t>
+  </si>
+  <si>
+    <t>Port C</t>
+  </si>
+  <si>
+    <t>0x23</t>
   </si>
 </sst>
 </file>
@@ -324,10 +330,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -593,10 +595,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="D2:E21"/>
+  <dimension ref="D2:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -647,13 +649,17 @@
       <c r="D8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D9" s="16"/>
-      <c r="E9" s="12"/>
     </row>
     <row r="10" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D10" s="16"/>
@@ -664,40 +670,40 @@
       <c r="E11" s="12"/>
     </row>
     <row r="12" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="16"/>
+      <c r="E12" s="12"/>
+    </row>
+    <row r="13" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D13" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="14"/>
-    </row>
-    <row r="13" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D13" s="2" t="s">
+      <c r="E13" s="14"/>
+    </row>
+    <row r="14" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D14" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E14" s="11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D14" s="2"/>
-      <c r="E14" s="12"/>
-    </row>
     <row r="15" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="2"/>
+      <c r="E15" s="12"/>
+    </row>
+    <row r="16" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D16" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E15" s="14"/>
-    </row>
-    <row r="16" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D16" s="5" t="s">
+      <c r="E16" s="14"/>
+    </row>
+    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D17" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="E17" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D17" s="16"/>
-      <c r="E17" s="12"/>
     </row>
     <row r="18" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D18" s="16"/>
@@ -711,21 +717,25 @@
       <c r="D20" s="16"/>
       <c r="E20" s="12"/>
     </row>
-    <row r="21" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D21" s="3" t="s">
+    <row r="21" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D21" s="16"/>
+      <c r="E21" s="12"/>
+    </row>
+    <row r="22" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D22" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E21" s="13"/>
+      <c r="E22" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="D3:E3"/>
-    <mergeCell ref="E16:E21"/>
-    <mergeCell ref="E13:E15"/>
-    <mergeCell ref="E8:E12"/>
+    <mergeCell ref="E17:E22"/>
+    <mergeCell ref="E14:E16"/>
+    <mergeCell ref="E9:E13"/>
     <mergeCell ref="E4:E5"/>
-    <mergeCell ref="D17:D20"/>
-    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="D18:D21"/>
+    <mergeCell ref="D10:D12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>